<commit_message>
corregido error en base de datos
</commit_message>
<xml_diff>
--- a/clase10/tpIntB/datos/datos.xlsx
+++ b/clase10/tpIntB/datos/datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\datos\zalo\cursos\argentinaPrograma\javaInicial\clase10\tpIntB\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D5F660-6A17-4CEC-8711-280D330A19A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DCE62C-1AE9-4EA2-88CA-E5702D6D67F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="1" r:id="rId1"/>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,16 +1843,16 @@
         <v>9</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C82" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,16 +1860,16 @@
         <v>9</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E83" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1877,16 +1877,16 @@
         <v>9</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E84" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1894,16 +1894,16 @@
         <v>9</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C85" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E85" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -1911,16 +1911,16 @@
         <v>9</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C86" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E86" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1928,16 +1928,16 @@
         <v>9</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C87" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E87" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,13 +1945,13 @@
         <v>9</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C88" s="1">
         <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
@@ -1962,16 +1962,16 @@
         <v>9</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C89" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E89" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1979,16 +1979,16 @@
         <v>9</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C90" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E90" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1996,16 +1996,16 @@
         <v>9</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C91" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3717,7 +3717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BECDD5-4DBF-4F19-8621-0412C57BCBD8}">
   <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+    <sheetView topLeftCell="A172" workbookViewId="0">
       <selection activeCell="D192" sqref="D192"/>
     </sheetView>
   </sheetViews>

</xml_diff>